<commit_message>
Agregando Cambios al Proyecto FInal: un scritp por Modelo, EDA datos
</commit_message>
<xml_diff>
--- a/Datos/Datos_Crudos.xlsx
+++ b/Datos/Datos_Crudos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\E$\ITAM_Maestria\03_Otono_2018\01 Regresión Avanzda\05 Proyecto Final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\E$\ITAM_Maestria\03_Otono_2018\01_Regresion_Avanzada\05_Proyecto_Final\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -9052,7 +9052,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>